<commit_message>
add N X Tree
</commit_message>
<xml_diff>
--- a/leetcode.xlsx
+++ b/leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\JetBrains\CLion 2018.2.5\Item_Set\clion_p1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804ADC0E-EA2A-41B4-ACB2-D4F082DD53A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A0C50-A1A5-4184-A3AA-25416698118A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5565" yWindow="1365" windowWidth="21630" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="680">
   <si>
     <t>题号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2746,6 +2746,42 @@
   </si>
   <si>
     <t>堆排序，细节是子母序，蛋疼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>递归，暂时没弄懂  也可以动态规划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L429</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L589</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N叉树的后序遍历</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L590</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N叉树的层序遍历</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N叉树的最大深度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L559</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N叉树的前序遍历</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3019,13 +3055,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3326,10 +3362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E302"/>
+  <dimension ref="A1:E305"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+      <selection activeCell="A245" sqref="A245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3360,13 +3396,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -3468,13 +3504,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="33" t="s">
         <v>507</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -3678,13 +3714,13 @@
       <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
@@ -4087,13 +4123,13 @@
       <c r="E60" s="6"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="31" t="s">
+      <c r="A61" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
@@ -4298,13 +4334,13 @@
       <c r="E79" s="6"/>
     </row>
     <row r="80" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="31" t="s">
+      <c r="A80" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="31"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
@@ -4453,13 +4489,13 @@
       <c r="E92" s="6"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A93" s="31" t="s">
+      <c r="A93" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B93" s="31"/>
-      <c r="C93" s="31"/>
-      <c r="D93" s="31"/>
-      <c r="E93" s="31"/>
+      <c r="B93" s="33"/>
+      <c r="C93" s="33"/>
+      <c r="D93" s="33"/>
+      <c r="E93" s="33"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="s">
@@ -4609,13 +4645,13 @@
       <c r="E106" s="6"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" s="31" t="s">
+      <c r="A107" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="B107" s="31"/>
-      <c r="C107" s="31"/>
-      <c r="D107" s="31"/>
-      <c r="E107" s="31"/>
+      <c r="B107" s="33"/>
+      <c r="C107" s="33"/>
+      <c r="D107" s="33"/>
+      <c r="E107" s="33"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
@@ -4758,13 +4794,13 @@
       <c r="E119" s="6"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="31" t="s">
+      <c r="A120" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="B120" s="31"/>
-      <c r="C120" s="31"/>
-      <c r="D120" s="31"/>
-      <c r="E120" s="31"/>
+      <c r="B120" s="33"/>
+      <c r="C120" s="33"/>
+      <c r="D120" s="33"/>
+      <c r="E120" s="33"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
@@ -4945,13 +4981,13 @@
       <c r="E134" s="6"/>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="31" t="s">
+      <c r="A135" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B135" s="31"/>
-      <c r="C135" s="31"/>
-      <c r="D135" s="31"/>
-      <c r="E135" s="31"/>
+      <c r="B135" s="33"/>
+      <c r="C135" s="33"/>
+      <c r="D135" s="33"/>
+      <c r="E135" s="33"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
@@ -5024,13 +5060,13 @@
       <c r="E141" s="6"/>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="31" t="s">
+      <c r="A142" s="33" t="s">
         <v>144</v>
       </c>
-      <c r="B142" s="31"/>
-      <c r="C142" s="31"/>
-      <c r="D142" s="31"/>
-      <c r="E142" s="31"/>
+      <c r="B142" s="33"/>
+      <c r="C142" s="33"/>
+      <c r="D142" s="33"/>
+      <c r="E142" s="33"/>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
@@ -5099,13 +5135,13 @@
       <c r="E148" s="6"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="31" t="s">
+      <c r="A149" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="B149" s="31"/>
-      <c r="C149" s="31"/>
-      <c r="D149" s="31"/>
-      <c r="E149" s="31"/>
+      <c r="B149" s="33"/>
+      <c r="C149" s="33"/>
+      <c r="D149" s="33"/>
+      <c r="E149" s="33"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="12" t="s">
@@ -5132,13 +5168,13 @@
       <c r="E151" s="6"/>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="31" t="s">
+      <c r="A152" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B152" s="31"/>
-      <c r="C152" s="31"/>
-      <c r="D152" s="31"/>
-      <c r="E152" s="31"/>
+      <c r="B152" s="33"/>
+      <c r="C152" s="33"/>
+      <c r="D152" s="33"/>
+      <c r="E152" s="33"/>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
@@ -5209,13 +5245,13 @@
       <c r="E158" s="6"/>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A159" s="31" t="s">
+      <c r="A159" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="B159" s="31"/>
-      <c r="C159" s="31"/>
-      <c r="D159" s="31"/>
-      <c r="E159" s="31"/>
+      <c r="B159" s="33"/>
+      <c r="C159" s="33"/>
+      <c r="D159" s="33"/>
+      <c r="E159" s="33"/>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
@@ -5262,13 +5298,13 @@
       <c r="E163" s="6"/>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A164" s="31" t="s">
+      <c r="A164" s="33" t="s">
         <v>530</v>
       </c>
-      <c r="B164" s="31"/>
-      <c r="C164" s="31"/>
-      <c r="D164" s="31"/>
-      <c r="E164" s="31"/>
+      <c r="B164" s="33"/>
+      <c r="C164" s="33"/>
+      <c r="D164" s="33"/>
+      <c r="E164" s="33"/>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
@@ -5323,13 +5359,13 @@
       <c r="E168" s="6"/>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A169" s="31" t="s">
+      <c r="A169" s="33" t="s">
         <v>523</v>
       </c>
-      <c r="B169" s="31"/>
-      <c r="C169" s="31"/>
-      <c r="D169" s="31"/>
-      <c r="E169" s="31"/>
+      <c r="B169" s="33"/>
+      <c r="C169" s="33"/>
+      <c r="D169" s="33"/>
+      <c r="E169" s="33"/>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
@@ -5459,13 +5495,13 @@
       <c r="E180" s="6"/>
     </row>
     <row r="181" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A181" s="31" t="s">
+      <c r="A181" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B181" s="31"/>
-      <c r="C181" s="31"/>
-      <c r="D181" s="31"/>
-      <c r="E181" s="31"/>
+      <c r="B181" s="33"/>
+      <c r="C181" s="33"/>
+      <c r="D181" s="33"/>
+      <c r="E181" s="33"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
@@ -5546,11 +5582,11 @@
       <c r="E187" s="6"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A188" s="32"/>
-      <c r="B188" s="32"/>
-      <c r="C188" s="32"/>
-      <c r="D188" s="32"/>
-      <c r="E188" s="33"/>
+      <c r="A188" s="31"/>
+      <c r="B188" s="31"/>
+      <c r="C188" s="31"/>
+      <c r="D188" s="31"/>
+      <c r="E188" s="32"/>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
@@ -5581,11 +5617,11 @@
       <c r="E190" s="6"/>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A191" s="32"/>
-      <c r="B191" s="32"/>
-      <c r="C191" s="32"/>
-      <c r="D191" s="32"/>
-      <c r="E191" s="33"/>
+      <c r="A191" s="31"/>
+      <c r="B191" s="31"/>
+      <c r="C191" s="31"/>
+      <c r="D191" s="31"/>
+      <c r="E191" s="32"/>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="12" t="s">
@@ -5666,11 +5702,11 @@
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A198" s="32"/>
-      <c r="B198" s="32"/>
-      <c r="C198" s="32"/>
-      <c r="D198" s="32"/>
-      <c r="E198" s="33"/>
+      <c r="A198" s="31"/>
+      <c r="B198" s="31"/>
+      <c r="C198" s="31"/>
+      <c r="D198" s="31"/>
+      <c r="E198" s="32"/>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="12" t="s">
@@ -5706,11 +5742,11 @@
       <c r="E201" s="6"/>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A202" s="32"/>
-      <c r="B202" s="32"/>
-      <c r="C202" s="32"/>
-      <c r="D202" s="32"/>
-      <c r="E202" s="33"/>
+      <c r="A202" s="31"/>
+      <c r="B202" s="31"/>
+      <c r="C202" s="31"/>
+      <c r="D202" s="31"/>
+      <c r="E202" s="32"/>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="12" t="s">
@@ -5763,13 +5799,13 @@
       <c r="E206" s="6"/>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A207" s="31" t="s">
+      <c r="A207" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="B207" s="31"/>
-      <c r="C207" s="31"/>
-      <c r="D207" s="31"/>
-      <c r="E207" s="31"/>
+      <c r="B207" s="33"/>
+      <c r="C207" s="33"/>
+      <c r="D207" s="33"/>
+      <c r="E207" s="33"/>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
@@ -5905,13 +5941,13 @@
       <c r="E218" s="6"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A219" s="31" t="s">
+      <c r="A219" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="B219" s="31"/>
-      <c r="C219" s="31"/>
-      <c r="D219" s="31"/>
-      <c r="E219" s="31"/>
+      <c r="B219" s="33"/>
+      <c r="C219" s="33"/>
+      <c r="D219" s="33"/>
+      <c r="E219" s="33"/>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="36" t="s">
@@ -6222,619 +6258,609 @@
       <c r="E243" s="6"/>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A244" s="34"/>
-      <c r="B244" s="34"/>
-      <c r="C244" s="34"/>
-      <c r="D244" s="34"/>
-      <c r="E244" s="35"/>
+      <c r="A244" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="C244" s="1"/>
+      <c r="D244" s="1"/>
+      <c r="E244" s="6"/>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A245" s="12" t="s">
-        <v>135</v>
+      <c r="A245" s="8" t="s">
+        <v>678</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>645</v>
+        <v>677</v>
       </c>
       <c r="C245" s="1"/>
-      <c r="D245" s="13"/>
-      <c r="E245" s="6" t="s">
-        <v>647</v>
-      </c>
+      <c r="D245" s="1"/>
+      <c r="E245" s="6"/>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="12" t="s">
-        <v>136</v>
+        <v>673</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>646</v>
+        <v>679</v>
       </c>
       <c r="C246" s="1"/>
-      <c r="D246" s="13"/>
-      <c r="E246" s="6" t="s">
-        <v>647</v>
-      </c>
+      <c r="D246" s="1"/>
+      <c r="E246" s="6"/>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="12" t="s">
-        <v>142</v>
+        <v>675</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>577</v>
+        <v>674</v>
       </c>
       <c r="C247" s="1"/>
-      <c r="D247" s="13" t="s">
-        <v>648</v>
-      </c>
+      <c r="D247" s="1"/>
       <c r="E247" s="6"/>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A248" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C248" s="1"/>
-      <c r="D248" s="13"/>
-      <c r="E248" s="6"/>
+      <c r="A248" s="34"/>
+      <c r="B248" s="34"/>
+      <c r="C248" s="34"/>
+      <c r="D248" s="34"/>
+      <c r="E248" s="35"/>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="12" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>146</v>
+        <v>645</v>
       </c>
       <c r="C249" s="1"/>
-      <c r="D249" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="E249" s="6"/>
+      <c r="D249" s="13"/>
+      <c r="E249" s="6" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="12" t="s">
-        <v>233</v>
+        <v>136</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>232</v>
+        <v>646</v>
       </c>
       <c r="C250" s="1"/>
-      <c r="D250" s="1" t="s">
-        <v>543</v>
-      </c>
-      <c r="E250" s="6"/>
+      <c r="D250" s="13"/>
+      <c r="E250" s="6" t="s">
+        <v>647</v>
+      </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="12" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>644</v>
-      </c>
+        <v>577</v>
+      </c>
+      <c r="C251" s="1"/>
       <c r="D251" s="13" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="E251" s="6"/>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="12" t="s">
-        <v>537</v>
+        <v>143</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>538</v>
+        <v>140</v>
       </c>
       <c r="C252" s="1"/>
-      <c r="D252" s="1" t="s">
-        <v>651</v>
-      </c>
+      <c r="D252" s="13"/>
       <c r="E252" s="6"/>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A253" s="32"/>
-      <c r="B253" s="32"/>
-      <c r="C253" s="32"/>
-      <c r="D253" s="32"/>
-      <c r="E253" s="33"/>
+      <c r="A253" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C253" s="1"/>
+      <c r="D253" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="E253" s="6"/>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="12" t="s">
-        <v>606</v>
-      </c>
-      <c r="B254" s="12" t="s">
-        <v>643</v>
-      </c>
-      <c r="C254" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C254" s="1"/>
+      <c r="D254" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="E254" s="6"/>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A255" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C255" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="D254" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="E254" s="6" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A255" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C255" s="1"/>
-      <c r="D255" s="1" t="s">
-        <v>582</v>
+      <c r="D255" s="13" t="s">
+        <v>652</v>
       </c>
       <c r="E255" s="6"/>
     </row>
-    <row r="256" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="12" t="s">
-        <v>137</v>
+        <v>537</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>633</v>
+        <v>538</v>
       </c>
       <c r="C256" s="1"/>
       <c r="D256" s="1" t="s">
-        <v>635</v>
+        <v>651</v>
       </c>
       <c r="E256" s="6"/>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A257" s="12" t="s">
-        <v>587</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>634</v>
-      </c>
-      <c r="C257" s="1"/>
-      <c r="D257" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="E257" s="23" t="s">
-        <v>636</v>
+      <c r="A257" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="B257" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A258" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B258" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C258" s="1"/>
-      <c r="D258" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="E258" s="6"/>
+      <c r="A258" s="31"/>
+      <c r="B258" s="31"/>
+      <c r="C258" s="31"/>
+      <c r="D258" s="31"/>
+      <c r="E258" s="32"/>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C259" s="1"/>
+        <v>606</v>
+      </c>
+      <c r="B259" s="12" t="s">
+        <v>643</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>644</v>
+      </c>
       <c r="D259" s="1" t="s">
         <v>582</v>
       </c>
       <c r="E259" s="6" t="s">
-        <v>639</v>
+        <v>605</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A260" s="12" t="s">
-        <v>202</v>
+      <c r="A260" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>200</v>
+        <v>124</v>
       </c>
       <c r="C260" s="1"/>
-      <c r="D260" s="1"/>
-      <c r="E260" s="6" t="s">
-        <v>639</v>
-      </c>
+      <c r="D260" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="E260" s="6"/>
     </row>
     <row r="261" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A261" s="12" t="s">
-        <v>640</v>
+        <v>137</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="C261" s="1"/>
-      <c r="D261" s="1"/>
-      <c r="E261" s="6" t="s">
-        <v>642</v>
-      </c>
+      <c r="D261" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="E261" s="6"/>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" s="12" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>593</v>
+        <v>634</v>
       </c>
       <c r="C262" s="1"/>
       <c r="D262" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="E262" s="6" t="s">
-        <v>642</v>
+      <c r="E262" s="23" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A263" s="12" t="s">
-        <v>590</v>
+      <c r="A263" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>591</v>
+        <v>192</v>
       </c>
       <c r="C263" s="1"/>
       <c r="D263" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="E263" s="6" t="s">
-        <v>637</v>
-      </c>
+      <c r="E263" s="6"/>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" s="12" t="s">
-        <v>586</v>
+        <v>201</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>585</v>
+        <v>199</v>
       </c>
       <c r="C264" s="1"/>
       <c r="D264" s="1" t="s">
         <v>582</v>
       </c>
       <c r="E264" s="6" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="265" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" s="12" t="s">
-        <v>588</v>
+        <v>202</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>589</v>
+        <v>200</v>
       </c>
       <c r="C265" s="1"/>
-      <c r="D265" s="1" t="s">
+      <c r="D265" s="1"/>
+      <c r="E265" s="6" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A266" s="12" t="s">
+        <v>640</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C266" s="1"/>
+      <c r="D266" s="1"/>
+      <c r="E266" s="6" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A267" s="12" t="s">
+        <v>592</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C267" s="1"/>
+      <c r="D267" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="E265" s="6" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A266" s="12" t="s">
-        <v>583</v>
-      </c>
-      <c r="B266" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="C266" s="1"/>
-      <c r="D266" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="E266" s="6" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A267" s="32"/>
-      <c r="B267" s="32"/>
-      <c r="C267" s="32"/>
-      <c r="D267" s="32"/>
-      <c r="E267" s="32"/>
+      <c r="E267" s="6" t="s">
+        <v>642</v>
+      </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A268" s="1" t="s">
-        <v>213</v>
+      <c r="A268" s="12" t="s">
+        <v>590</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>214</v>
+        <v>591</v>
       </c>
       <c r="C268" s="1"/>
       <c r="D268" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="E268" s="6"/>
+        <v>582</v>
+      </c>
+      <c r="E268" s="6" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" s="12" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="C269" s="1"/>
       <c r="D269" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="E269" s="6"/>
-    </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A270" s="31" t="s">
-        <v>565</v>
-      </c>
-      <c r="B270" s="31"/>
-      <c r="C270" s="31"/>
-      <c r="D270" s="31"/>
-      <c r="E270" s="31"/>
+        <v>582</v>
+      </c>
+      <c r="E269" s="6" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A270" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="C270" s="1"/>
+      <c r="D270" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="E270" s="6" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A271" s="1" t="s">
-        <v>211</v>
+      <c r="A271" s="12" t="s">
+        <v>583</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>613</v>
+        <v>584</v>
       </c>
       <c r="C271" s="1"/>
       <c r="D271" s="1" t="s">
-        <v>616</v>
-      </c>
-      <c r="E271" s="6"/>
+        <v>582</v>
+      </c>
+      <c r="E271" s="6" t="s">
+        <v>638</v>
+      </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A272" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="C272" s="1"/>
-      <c r="D272" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="E272" s="6"/>
-    </row>
-    <row r="273" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="A273" s="12" t="s">
-        <v>562</v>
+      <c r="A272" s="31"/>
+      <c r="B272" s="31"/>
+      <c r="C272" s="31"/>
+      <c r="D272" s="31"/>
+      <c r="E272" s="31"/>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A273" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>564</v>
+        <v>214</v>
       </c>
       <c r="C273" s="1"/>
       <c r="D273" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="E273" s="6" t="s">
-        <v>563</v>
-      </c>
+        <v>594</v>
+      </c>
+      <c r="E273" s="6"/>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A274" s="32"/>
-      <c r="B274" s="32"/>
-      <c r="C274" s="32"/>
-      <c r="D274" s="32"/>
-      <c r="E274" s="33"/>
-    </row>
-    <row r="275" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A275" s="12" t="s">
-        <v>372</v>
-      </c>
-      <c r="B275" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="C275" s="1"/>
-      <c r="D275" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="E275" s="6"/>
+      <c r="A274" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="C274" s="1"/>
+      <c r="D274" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="E274" s="6"/>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A275" s="33" t="s">
+        <v>565</v>
+      </c>
+      <c r="B275" s="33"/>
+      <c r="C275" s="33"/>
+      <c r="D275" s="33"/>
+      <c r="E275" s="33"/>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>241</v>
+        <v>613</v>
       </c>
       <c r="C276" s="1"/>
       <c r="D276" s="1" t="s">
-        <v>542</v>
+        <v>616</v>
       </c>
       <c r="E276" s="6"/>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" s="12" t="s">
-        <v>540</v>
+        <v>212</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>541</v>
+        <v>614</v>
       </c>
       <c r="C277" s="1"/>
       <c r="D277" s="1" t="s">
-        <v>542</v>
+        <v>615</v>
       </c>
       <c r="E277" s="6"/>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A278" s="34"/>
-      <c r="B278" s="34"/>
-      <c r="C278" s="34"/>
-      <c r="D278" s="34"/>
-      <c r="E278" s="35"/>
+    <row r="278" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A278" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="C278" s="1"/>
+      <c r="D278" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="E278" s="6" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A279" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="B279" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="C279" s="1"/>
-      <c r="D279" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="E279" s="6"/>
-    </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A279" s="31"/>
+      <c r="B279" s="31"/>
+      <c r="C279" s="31"/>
+      <c r="D279" s="31"/>
+      <c r="E279" s="32"/>
+    </row>
+    <row r="280" spans="1:5" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A280" s="12" t="s">
-        <v>149</v>
+        <v>372</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>547</v>
+        <v>611</v>
       </c>
       <c r="C280" s="1"/>
       <c r="D280" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E280" s="6"/>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="B281" s="1" t="s">
-        <v>545</v>
+        <v>241</v>
       </c>
       <c r="C281" s="1"/>
       <c r="D281" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E281" s="6"/>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" s="12" t="s">
-        <v>466</v>
+        <v>540</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="C282" s="1"/>
       <c r="D282" s="1" t="s">
-        <v>609</v>
+        <v>542</v>
       </c>
       <c r="E282" s="6"/>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A283" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C283" s="1"/>
-      <c r="D283" s="1" t="s">
-        <v>609</v>
-      </c>
-      <c r="E283" s="6" t="s">
-        <v>610</v>
-      </c>
+      <c r="A283" s="34"/>
+      <c r="B283" s="34"/>
+      <c r="C283" s="34"/>
+      <c r="D283" s="34"/>
+      <c r="E283" s="35"/>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A284" s="12" t="s">
-        <v>464</v>
+      <c r="A284" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="C284" s="1"/>
       <c r="D284" s="1" t="s">
-        <v>543</v>
+        <v>608</v>
       </c>
       <c r="E284" s="6"/>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" s="12" t="s">
-        <v>455</v>
+        <v>149</v>
       </c>
       <c r="B285" s="1" t="s">
-        <v>456</v>
+        <v>547</v>
       </c>
       <c r="C285" s="1"/>
       <c r="D285" s="1" t="s">
-        <v>612</v>
+        <v>543</v>
       </c>
       <c r="E285" s="6"/>
     </row>
-    <row r="286" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A286" s="31" t="s">
-        <v>604</v>
-      </c>
-      <c r="B286" s="31"/>
-      <c r="C286" s="31"/>
-      <c r="D286" s="31"/>
-      <c r="E286" s="31"/>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A286" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C286" s="1"/>
+      <c r="D286" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="E286" s="6"/>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A287" s="1" t="s">
-        <v>45</v>
+      <c r="A287" s="12" t="s">
+        <v>466</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>46</v>
+        <v>548</v>
       </c>
       <c r="C287" s="1"/>
-      <c r="D287" s="24" t="s">
-        <v>549</v>
+      <c r="D287" s="1" t="s">
+        <v>609</v>
       </c>
       <c r="E287" s="6"/>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A288" s="1" t="s">
-        <v>55</v>
+      <c r="A288" s="12" t="s">
+        <v>465</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>56</v>
+        <v>546</v>
       </c>
       <c r="C288" s="1"/>
-      <c r="D288" s="24" t="s">
-        <v>549</v>
-      </c>
-      <c r="E288" s="6"/>
+      <c r="D288" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="E288" s="6" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A289" s="12" t="s">
-        <v>560</v>
+        <v>464</v>
       </c>
       <c r="B289" s="1" t="s">
-        <v>561</v>
+        <v>544</v>
       </c>
       <c r="C289" s="1"/>
-      <c r="D289" s="24" t="s">
-        <v>549</v>
+      <c r="D289" s="1" t="s">
+        <v>543</v>
       </c>
       <c r="E289" s="6"/>
     </row>
-    <row r="290" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A290" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B290" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C290" s="25"/>
-      <c r="D290" s="24" t="s">
-        <v>600</v>
-      </c>
-      <c r="E290" s="26"/>
-    </row>
-    <row r="291" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A291" s="25" t="s">
-        <v>554</v>
-      </c>
-      <c r="B291" s="25" t="s">
-        <v>555</v>
-      </c>
-      <c r="C291" s="25"/>
-      <c r="D291" s="24" t="s">
-        <v>549</v>
-      </c>
-      <c r="E291" s="26"/>
+    <row r="290" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A290" s="12" t="s">
+        <v>455</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C290" s="1"/>
+      <c r="D290" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="E290" s="6"/>
+    </row>
+    <row r="291" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A291" s="33" t="s">
+        <v>604</v>
+      </c>
+      <c r="B291" s="33"/>
+      <c r="C291" s="33"/>
+      <c r="D291" s="33"/>
+      <c r="E291" s="33"/>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A292" s="12" t="s">
-        <v>556</v>
-      </c>
-      <c r="B292" s="12" t="s">
-        <v>557</v>
+      <c r="A292" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C292" s="1"/>
       <c r="D292" s="24" t="s">
@@ -6844,10 +6870,10 @@
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A293" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B293" s="12" t="s">
-        <v>72</v>
+        <v>55</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="C293" s="1"/>
       <c r="D293" s="24" t="s">
@@ -6857,10 +6883,10 @@
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A294" s="12" t="s">
-        <v>552</v>
-      </c>
-      <c r="B294" s="12" t="s">
-        <v>553</v>
+        <v>560</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>561</v>
       </c>
       <c r="C294" s="1"/>
       <c r="D294" s="24" t="s">
@@ -6868,38 +6894,38 @@
       </c>
       <c r="E294" s="6"/>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A295" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="B295" s="12" t="s">
-        <v>437</v>
-      </c>
-      <c r="C295" s="1"/>
+    <row r="295" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B295" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C295" s="25"/>
       <c r="D295" s="24" t="s">
-        <v>549</v>
-      </c>
-      <c r="E295" s="6"/>
-    </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A296" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="B296" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="C296" s="1"/>
+        <v>600</v>
+      </c>
+      <c r="E295" s="26"/>
+    </row>
+    <row r="296" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A296" s="25" t="s">
+        <v>554</v>
+      </c>
+      <c r="B296" s="25" t="s">
+        <v>555</v>
+      </c>
+      <c r="C296" s="25"/>
       <c r="D296" s="24" t="s">
         <v>549</v>
       </c>
-      <c r="E296" s="6"/>
+      <c r="E296" s="26"/>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A297" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B297" s="1" t="s">
-        <v>109</v>
+      <c r="A297" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="B297" s="12" t="s">
+        <v>557</v>
       </c>
       <c r="C297" s="1"/>
       <c r="D297" s="24" t="s">
@@ -6908,11 +6934,11 @@
       <c r="E297" s="6"/>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A298" s="12" t="s">
-        <v>558</v>
-      </c>
-      <c r="B298" s="1" t="s">
-        <v>559</v>
+      <c r="A298" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B298" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="C298" s="1"/>
       <c r="D298" s="24" t="s">
@@ -6922,10 +6948,10 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A299" s="12" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B299" s="12" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C299" s="1"/>
       <c r="D299" s="24" t="s">
@@ -6934,40 +6960,80 @@
       <c r="E299" s="6"/>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A300" s="28"/>
-      <c r="B300" s="28"/>
-      <c r="C300" s="28"/>
-      <c r="D300" s="28"/>
-      <c r="E300" s="29"/>
+      <c r="A300" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B300" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="C300" s="1"/>
+      <c r="D300" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="E300" s="6"/>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A301" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B301" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="C301" s="1"/>
+      <c r="D301" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="E301" s="6"/>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A302" s="5" t="s">
-        <v>653</v>
-      </c>
-      <c r="B302" s="5" t="s">
-        <v>654</v>
-      </c>
+      <c r="A302" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C302" s="1"/>
+      <c r="D302" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="E302" s="6"/>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A303" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C303" s="1"/>
+      <c r="D303" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="E303" s="6"/>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A304" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="B304" s="12" t="s">
+        <v>551</v>
+      </c>
+      <c r="C304" s="1"/>
+      <c r="D304" s="24" t="s">
+        <v>549</v>
+      </c>
+      <c r="E304" s="6"/>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A305" s="28"/>
+      <c r="B305" s="28"/>
+      <c r="C305" s="28"/>
+      <c r="D305" s="28"/>
+      <c r="E305" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="A191:E191"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A202:E202"/>
-    <mergeCell ref="A274:E274"/>
-    <mergeCell ref="A278:E278"/>
-    <mergeCell ref="A267:E267"/>
-    <mergeCell ref="A159:E159"/>
-    <mergeCell ref="A270:E270"/>
-    <mergeCell ref="A219:E219"/>
-    <mergeCell ref="A220:E220"/>
-    <mergeCell ref="A207:E207"/>
-    <mergeCell ref="E231:E232"/>
-    <mergeCell ref="A236:E236"/>
-    <mergeCell ref="A244:E244"/>
-    <mergeCell ref="A253:E253"/>
-    <mergeCell ref="E225:E227"/>
-    <mergeCell ref="A286:E286"/>
+    <mergeCell ref="A291:E291"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A169:E169"/>
     <mergeCell ref="A93:E93"/>
@@ -6983,6 +7049,23 @@
     <mergeCell ref="A142:E142"/>
     <mergeCell ref="A152:E152"/>
     <mergeCell ref="A188:E188"/>
+    <mergeCell ref="A283:E283"/>
+    <mergeCell ref="A272:E272"/>
+    <mergeCell ref="A159:E159"/>
+    <mergeCell ref="A275:E275"/>
+    <mergeCell ref="A219:E219"/>
+    <mergeCell ref="A220:E220"/>
+    <mergeCell ref="A207:E207"/>
+    <mergeCell ref="E231:E232"/>
+    <mergeCell ref="A236:E236"/>
+    <mergeCell ref="A248:E248"/>
+    <mergeCell ref="A258:E258"/>
+    <mergeCell ref="E225:E227"/>
+    <mergeCell ref="A191:E191"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A202:E202"/>
+    <mergeCell ref="A279:E279"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>